<commit_message>
updated expression schema and disease schema
</commit_message>
<xml_diff>
--- a/doc/json_schema_migration_from_1.1_to_1.2.xlsx
+++ b/doc/json_schema_migration_from_1.1_to_1.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="164">
   <si>
     <t>Table 1. Types of target-disease 'evidence chains': this field needs to be specified in .type field in the schema</t>
   </si>
@@ -502,6 +502,12 @@
   </si>
   <si>
     <t>Table 2. Types of 'evidence' objects for linking 2 entities and their corresponding 'evidence chain'</t>
+  </si>
+  <si>
+    <t>Control sample</t>
+  </si>
+  <si>
+    <t>Test sample</t>
   </si>
 </sst>
 </file>
@@ -725,9 +731,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -745,9 +748,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -760,11 +760,81 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -797,6 +867,69 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -833,153 +966,26 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:B11" totalsRowShown="0" headerRowDxfId="1" dataDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:B11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <tableColumns count="2">
-    <tableColumn id="1" name="CTTV data project" dataDxfId="12"/>
-    <tableColumn id="2" name=".type field in schema" dataDxfId="11"/>
+    <tableColumn id="1" name="CTTV data project" dataDxfId="7"/>
+    <tableColumn id="2" name=".type field in schema" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A15:B24" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A15:B24" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <tableColumns count="2">
-    <tableColumn id="1" name="Evidence chain type (.type)" dataDxfId="7"/>
-    <tableColumn id="2" name="EVIDENCE_OBJECT" dataDxfId="6"/>
+    <tableColumn id="1" name="Evidence chain type (.type)" dataDxfId="1"/>
+    <tableColumn id="2" name="EVIDENCE_OBJECT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1270,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1285,107 +1291,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="20"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="30">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="33.75" customHeight="1">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3">
@@ -1394,98 +1400,98 @@
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="21" customHeight="1">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:4" ht="45">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1494,24 +1500,24 @@
       <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:4" ht="30" customHeight="1">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="24" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1798,260 +1804,276 @@
     <row r="51" spans="1:4">
       <c r="A51" s="7"/>
       <c r="B51" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>106</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="7"/>
       <c r="B52" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>109</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="7"/>
       <c r="B53" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D55" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9" t="s">
+    <row r="56" spans="1:4">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C56" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D56" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="45">
-      <c r="A55" s="13" t="s">
+    <row r="57" spans="1:4" ht="45">
+      <c r="A57" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B57" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C57" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D57" s="13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="30">
-      <c r="A56" s="7" t="s">
+    <row r="58" spans="1:4" ht="30">
+      <c r="A58" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D58" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9" t="s">
+    <row r="59" spans="1:4">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C59" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D57" s="9" t="s">
+      <c r="D59" s="9" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="7" t="s">
+    <row r="60" spans="1:4">
+      <c r="A60" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B60" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C60" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="D58" s="10" t="s">
+      <c r="D60" s="10" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="7"/>
-      <c r="B59" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="7"/>
-      <c r="B60" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="7"/>
       <c r="B61" s="10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>134</v>
+      <c r="A62" s="7"/>
+      <c r="B62" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="7"/>
       <c r="B63" s="10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="9"/>
       <c r="B64" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="7"/>
+      <c r="B65" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="9"/>
+      <c r="B66" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D66" s="9" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="10" t="s">
+    <row r="67" spans="1:4">
+      <c r="A67" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B67" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="C67" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="D67" s="13" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="7"/>
-      <c r="B66" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="7"/>
-      <c r="B67" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="7"/>
       <c r="B68" s="10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>149</v>
+        <v>70</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="7"/>
-      <c r="B69" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>153</v>
+      <c r="B69" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="7"/>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="7"/>
+      <c r="B71" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C72" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D72" s="7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9" t="s">
+    <row r="73" spans="1:4">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C71" s="9" t="s">
+      <c r="C73" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D73" s="9" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added drug and genetics fields
</commit_message>
<xml_diff>
--- a/doc/json_schema_migration_from_1.1_to_1.2.xlsx
+++ b/doc/json_schema_migration_from_1.1_to_1.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="175">
   <si>
     <t>Table 1. Types of target-disease 'evidence chains': this field needs to be specified in .type field in the schema</t>
   </si>
@@ -540,7 +540,7 @@
     <t>.evidence.expression.log2_fold_change.rank.sample_size</t>
   </si>
   <si>
-    <t>affected_pathways</t>
+    <t>affected_pathways_string</t>
   </si>
 </sst>
 </file>
@@ -1319,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1331,7 +1331,7 @@
     <col min="2" max="2" width="61.85546875" customWidth="1"/>
     <col min="3" max="3" width="77.42578125" customWidth="1"/>
     <col min="4" max="4" width="64.85546875" customWidth="1"/>
-    <col min="5" max="6" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:8">
       <c r="A17" s="14" t="s">
         <v>14</v>
       </c>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:8">
       <c r="A18" s="14" t="s">
         <v>9</v>
       </c>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="45">
+    <row r="19" spans="1:8" ht="45">
       <c r="A19" s="14" t="s">
         <v>24</v>
       </c>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:8">
       <c r="A20" s="14" t="s">
         <v>7</v>
       </c>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:8">
       <c r="A21" s="14" t="s">
         <v>7</v>
       </c>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:8">
       <c r="A22" s="14" t="s">
         <v>18</v>
       </c>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:8">
       <c r="A23" s="14" t="s">
         <v>18</v>
       </c>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:8">
       <c r="A24" s="16" t="s">
         <v>18</v>
       </c>
@@ -1539,11 +1539,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:8">
       <c r="A25" s="5"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1">
+    <row r="26" spans="1:8" ht="30" customHeight="1">
       <c r="A26" s="28" t="s">
         <v>31</v>
       </c>
@@ -1552,7 +1552,7 @@
       <c r="D26" s="28"/>
       <c r="E26" s="25"/>
     </row>
-    <row r="27" spans="1:6" ht="95.25">
+    <row r="27" spans="1:8" ht="138.75">
       <c r="A27" s="23" t="s">
         <v>32</v>
       </c>
@@ -1566,13 +1566,19 @@
         <v>35</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="F27" s="25" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="6" t="s">
         <v>36</v>
       </c>
@@ -1587,8 +1593,10 @@
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="26"/>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="7"/>
       <c r="B29" s="6" t="s">
         <v>40</v>
@@ -1601,8 +1609,10 @@
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="26"/>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="7"/>
       <c r="B30" s="6" t="s">
         <v>43</v>
@@ -1615,8 +1625,10 @@
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="26"/>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="7"/>
       <c r="B31" s="6" t="s">
         <v>46</v>
@@ -1629,8 +1641,10 @@
       </c>
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="7"/>
       <c r="B32" s="6" t="s">
         <v>49</v>
@@ -1641,8 +1655,9 @@
       <c r="D32" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" s="26"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="7"/>
       <c r="B33" s="8" t="s">
         <v>52</v>
@@ -1653,8 +1668,9 @@
       <c r="D33" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" s="26"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="7"/>
       <c r="B34" s="6" t="s">
         <v>54</v>
@@ -1667,8 +1683,10 @@
       </c>
       <c r="E34" s="26"/>
       <c r="F34" s="26"/>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="7"/>
       <c r="B35" s="7" t="s">
         <v>57</v>
@@ -1681,8 +1699,10 @@
       </c>
       <c r="E35" s="26"/>
       <c r="F35" s="26"/>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="7"/>
       <c r="B36" s="7" t="s">
         <v>159</v>
@@ -1695,8 +1715,10 @@
       </c>
       <c r="E36" s="26"/>
       <c r="F36" s="26"/>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="7"/>
       <c r="B37" s="6" t="s">
         <v>161</v>
@@ -1709,7 +1731,7 @@
       </c>
       <c r="E37" s="26"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:8">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
         <v>162</v>
@@ -1722,7 +1744,7 @@
       </c>
       <c r="E38" s="26"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:8">
       <c r="A39" s="7"/>
       <c r="B39" s="6" t="s">
         <v>61</v>
@@ -1735,8 +1757,10 @@
       </c>
       <c r="E39" s="26"/>
       <c r="F39" s="26"/>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="7"/>
       <c r="B40" s="6" t="s">
         <v>64</v>
@@ -1749,8 +1773,10 @@
       </c>
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="7"/>
       <c r="B41" s="6" t="s">
         <v>67</v>
@@ -1763,8 +1789,10 @@
       </c>
       <c r="E41" s="26"/>
       <c r="F41" s="26"/>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="7"/>
       <c r="B42" s="6" t="s">
         <v>70</v>
@@ -1777,8 +1805,10 @@
       </c>
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="7"/>
       <c r="B43" s="6" t="s">
         <v>73</v>
@@ -1790,8 +1820,10 @@
         <v>75</v>
       </c>
       <c r="E43" s="26"/>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43" s="20"/>
+      <c r="H43" s="26"/>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="7"/>
       <c r="B44" s="6" t="s">
         <v>76</v>
@@ -1803,8 +1835,10 @@
         <v>78</v>
       </c>
       <c r="F44" s="26"/>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44" s="20"/>
+      <c r="H44" s="26"/>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="7"/>
       <c r="B45" s="6" t="s">
         <v>79</v>
@@ -1815,8 +1849,9 @@
       <c r="D45" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="30">
+      <c r="G45" s="20"/>
+    </row>
+    <row r="46" spans="1:8" ht="30">
       <c r="A46" s="7"/>
       <c r="B46" s="6" t="s">
         <v>82</v>
@@ -1827,8 +1862,9 @@
       <c r="D46" s="11" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46" s="20"/>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="7"/>
       <c r="B47" s="6" t="s">
         <v>85</v>
@@ -1840,8 +1876,10 @@
         <v>87</v>
       </c>
       <c r="F47" s="26"/>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="7"/>
       <c r="B48" s="6" t="s">
         <v>88</v>
@@ -1854,8 +1892,10 @@
       </c>
       <c r="E48" s="26"/>
       <c r="F48" s="26"/>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="7"/>
       <c r="B49" s="6" t="s">
         <v>91</v>
@@ -1867,8 +1907,10 @@
         <v>93</v>
       </c>
       <c r="F49" s="26"/>
-    </row>
-    <row r="50" spans="1:6" ht="30">
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+    </row>
+    <row r="50" spans="1:8" ht="30">
       <c r="A50" s="7"/>
       <c r="B50" s="6" t="s">
         <v>94</v>
@@ -1880,7 +1922,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="30">
+    <row r="51" spans="1:8" ht="30">
       <c r="A51" s="9"/>
       <c r="B51" s="8" t="s">
         <v>97</v>
@@ -1892,7 +1934,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:8">
       <c r="A52" s="7" t="s">
         <v>9</v>
       </c>
@@ -1907,7 +1949,7 @@
       </c>
       <c r="E52" s="26"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:8">
       <c r="A53" s="7"/>
       <c r="B53" s="7" t="s">
         <v>102</v>
@@ -1920,7 +1962,7 @@
       </c>
       <c r="E53" s="26"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:8">
       <c r="A54" s="7"/>
       <c r="B54" s="7" t="s">
         <v>169</v>
@@ -1933,7 +1975,7 @@
       </c>
       <c r="E54" s="26"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:8">
       <c r="A55" s="7"/>
       <c r="B55" s="7" t="s">
         <v>165</v>
@@ -1946,7 +1988,7 @@
       </c>
       <c r="E55" s="26"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:8">
       <c r="A56" s="7"/>
       <c r="B56" s="7" t="s">
         <v>170</v>
@@ -1959,7 +2001,7 @@
       </c>
       <c r="E56" s="26"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:8">
       <c r="A57" s="7"/>
       <c r="B57" s="7" t="s">
         <v>166</v>
@@ -1972,7 +2014,7 @@
       </c>
       <c r="E57" s="26"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:8">
       <c r="A58" s="7"/>
       <c r="B58" s="7" t="s">
         <v>158</v>
@@ -1985,7 +2027,7 @@
       </c>
       <c r="E58" s="26"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:8">
       <c r="A59" s="7"/>
       <c r="B59" s="7" t="s">
         <v>73</v>
@@ -1998,7 +2040,7 @@
       </c>
       <c r="E59" s="26"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:8">
       <c r="A60" s="9"/>
       <c r="B60" s="9" t="s">
         <v>108</v>
@@ -2011,7 +2053,7 @@
       </c>
       <c r="E60" s="26"/>
     </row>
-    <row r="61" spans="1:6" ht="45">
+    <row r="61" spans="1:8" ht="45">
       <c r="A61" s="13" t="s">
         <v>111</v>
       </c>
@@ -2026,7 +2068,7 @@
       </c>
       <c r="F61" s="26"/>
     </row>
-    <row r="62" spans="1:6" ht="30">
+    <row r="62" spans="1:8" ht="30">
       <c r="A62" s="7" t="s">
         <v>18</v>
       </c>
@@ -2040,7 +2082,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:8">
       <c r="A63" s="9"/>
       <c r="B63" s="9" t="s">
         <v>118</v>
@@ -2052,7 +2094,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:8">
       <c r="A64" s="7" t="s">
         <v>14</v>
       </c>
@@ -2065,8 +2107,9 @@
       <c r="D64" s="10" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="G64" s="26"/>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="7"/>
       <c r="B65" s="10" t="s">
         <v>123</v>
@@ -2077,8 +2120,9 @@
       <c r="D65" s="10" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="G65" s="26"/>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="7"/>
       <c r="B66" s="10" t="s">
         <v>125</v>
@@ -2089,8 +2133,9 @@
       <c r="D66" s="10" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="G66" s="26"/>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="7"/>
       <c r="B67" s="10" t="s">
         <v>128</v>
@@ -2101,8 +2146,9 @@
       <c r="D67" s="10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="G67" s="26"/>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="9"/>
       <c r="B68" s="9" t="s">
         <v>131</v>
@@ -2113,8 +2159,9 @@
       <c r="D68" s="9" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="G68" s="26"/>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="7"/>
       <c r="B69" s="10" t="s">
         <v>133</v>
@@ -2125,8 +2172,9 @@
       <c r="D69" s="10" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="G69" s="26"/>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="9"/>
       <c r="B70" s="9" t="s">
         <v>136</v>
@@ -2137,8 +2185,9 @@
       <c r="D70" s="9" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="G70" s="26"/>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="10" t="s">
         <v>7</v>
       </c>
@@ -2151,8 +2200,9 @@
       <c r="D71" s="13" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="H71" s="26"/>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="7"/>
       <c r="B72" s="10" t="s">
         <v>140</v>
@@ -2163,8 +2213,9 @@
       <c r="D72" s="10" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="H72" s="26"/>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="7"/>
       <c r="B73" s="9" t="s">
         <v>142</v>
@@ -2175,8 +2226,9 @@
       <c r="D73" s="9" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="H73" s="26"/>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="7"/>
       <c r="B74" s="10" t="s">
         <v>144</v>
@@ -2187,8 +2239,9 @@
       <c r="D74" s="10" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="H74" s="26"/>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="7"/>
       <c r="B75" s="10" t="s">
         <v>147</v>
@@ -2199,8 +2252,9 @@
       <c r="D75" s="10" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="H75" s="26"/>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="7"/>
       <c r="B76" s="7" t="s">
         <v>150</v>
@@ -2211,8 +2265,9 @@
       <c r="D76" s="7" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="H76" s="26"/>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="9"/>
       <c r="B77" s="9" t="s">
         <v>153</v>
@@ -2223,6 +2278,7 @@
       <c r="D77" s="9" t="s">
         <v>155</v>
       </c>
+      <c r="H77" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
added new drug fields
</commit_message>
<xml_diff>
--- a/doc/json_schema_migration_from_1.1_to_1.2.xlsx
+++ b/doc/json_schema_migration_from_1.1_to_1.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="183">
   <si>
     <t>Table 1. Types of target-disease 'evidence chains': this field needs to be specified in .type field in the schema</t>
   </si>
@@ -423,9 +423,6 @@
     <t>.evidence.evidence_chain[0].evidence.experiment_specific.name</t>
   </si>
   <si>
-    <t>.drug.name</t>
-  </si>
-  <si>
     <t>Drug ID</t>
   </si>
   <si>
@@ -547,6 +544,27 @@
   </si>
   <si>
     <t>=1</t>
+  </si>
+  <si>
+    <t>.drug.max_phase_for_all_diseases</t>
+  </si>
+  <si>
+    <t>Maximum phase for THIS disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .evidence.drug2clinic.max_phase_for_disease</t>
+  </si>
+  <si>
+    <t>Maximum phase for ALL diseases</t>
+  </si>
+  <si>
+    <t>Molecule type</t>
+  </si>
+  <si>
+    <t>.drug.molecule_type</t>
+  </si>
+  <si>
+    <t>.drug.molecule_name</t>
   </si>
 </sst>
 </file>
@@ -818,12 +836,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -833,6 +845,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1349,10 +1367,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1462,10 +1480,10 @@
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="33.75" customHeight="1">
-      <c r="A12" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="B12" s="26"/>
+      <c r="A12" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="33"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3">
@@ -1474,10 +1492,10 @@
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="21" customHeight="1">
-      <c r="A14" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="B14" s="27"/>
+      <c r="A14" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="34"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3">
@@ -1601,25 +1619,25 @@
       <c r="D27" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="F27" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="G27" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="J27" s="29" t="s">
+      <c r="J27" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="29" t="s">
+      <c r="K27" s="27" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1636,13 +1654,13 @@
       <c r="D28" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="7"/>
@@ -1655,13 +1673,13 @@
       <c r="D29" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="7"/>
@@ -1674,13 +1692,13 @@
       <c r="D30" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="7"/>
@@ -1693,13 +1711,13 @@
       <c r="D31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="7"/>
@@ -1712,7 +1730,7 @@
       <c r="D32" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G32" s="28"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="7"/>
@@ -1725,13 +1743,13 @@
       <c r="D33" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="7"/>
@@ -1744,13 +1762,13 @@
       <c r="D34" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="7"/>
@@ -1763,64 +1781,64 @@
       <c r="D35" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="7"/>
       <c r="B36" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
+        <v>159</v>
+      </c>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="7"/>
       <c r="B37" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="E37" s="28"/>
+        <v>162</v>
+      </c>
+      <c r="E37" s="26"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E38" s="32"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
+        <v>163</v>
+      </c>
+      <c r="E38" s="30"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="7"/>
@@ -1833,13 +1851,13 @@
       <c r="D39" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="7"/>
@@ -1852,13 +1870,13 @@
       <c r="D40" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="7"/>
@@ -1871,13 +1889,13 @@
       <c r="D41" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="7"/>
@@ -1890,13 +1908,13 @@
       <c r="D42" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="7"/>
@@ -1909,7 +1927,7 @@
       <c r="D43" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="28"/>
+      <c r="E43" s="26"/>
       <c r="G43" s="25"/>
       <c r="H43" s="25"/>
       <c r="J43" s="25"/>
@@ -1925,13 +1943,13 @@
       <c r="D44" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F44" s="33" t="s">
-        <v>176</v>
+      <c r="F44" s="31" t="s">
+        <v>175</v>
       </c>
       <c r="G44" s="25"/>
       <c r="H44" s="25"/>
-      <c r="I44" s="33" t="s">
-        <v>176</v>
+      <c r="I44" s="31" t="s">
+        <v>175</v>
       </c>
       <c r="J44" s="25"/>
     </row>
@@ -1976,12 +1994,12 @@
       <c r="D47" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
-      <c r="K47" s="28"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="7"/>
@@ -1994,13 +2012,13 @@
       <c r="D48" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="28"/>
-      <c r="K48" s="28"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="7"/>
@@ -2013,12 +2031,12 @@
       <c r="D49" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
     </row>
     <row r="50" spans="1:11" ht="30">
       <c r="A50" s="7"/>
@@ -2031,8 +2049,8 @@
       <c r="D50" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
     </row>
     <row r="51" spans="1:11" ht="30">
       <c r="A51" s="9"/>
@@ -2045,13 +2063,13 @@
       <c r="D51" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="30"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="28"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="7" t="s">
@@ -2066,7 +2084,7 @@
       <c r="D52" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E52" s="28"/>
+      <c r="E52" s="26"/>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="7"/>
@@ -2079,72 +2097,72 @@
       <c r="D53" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="28"/>
+      <c r="E53" s="26"/>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="7"/>
       <c r="B54" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>105</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E54" s="28"/>
+        <v>170</v>
+      </c>
+      <c r="E54" s="26"/>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="7"/>
       <c r="B55" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E55" s="28"/>
+        <v>171</v>
+      </c>
+      <c r="E55" s="26"/>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="7"/>
       <c r="B56" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E56" s="28"/>
+        <v>172</v>
+      </c>
+      <c r="E56" s="26"/>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="7"/>
       <c r="B57" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E57" s="28"/>
+        <v>166</v>
+      </c>
+      <c r="E57" s="26"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="7"/>
       <c r="B58" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E58" s="28"/>
+        <v>167</v>
+      </c>
+      <c r="E58" s="26"/>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="7"/>
@@ -2157,7 +2175,7 @@
       <c r="D59" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E59" s="28"/>
+      <c r="E59" s="26"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="9"/>
@@ -2170,13 +2188,13 @@
       <c r="D60" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E60" s="32"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="30"/>
-      <c r="J60" s="30"/>
-      <c r="K60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="28"/>
+      <c r="I60" s="28"/>
+      <c r="J60" s="28"/>
+      <c r="K60" s="28"/>
     </row>
     <row r="61" spans="1:11" ht="45">
       <c r="A61" s="13" t="s">
@@ -2191,13 +2209,13 @@
       <c r="D61" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E61" s="31"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="31"/>
-      <c r="H61" s="31"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="31"/>
-      <c r="K61" s="31"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="32"/>
+      <c r="J61" s="29"/>
+      <c r="K61" s="29"/>
     </row>
     <row r="62" spans="1:11" ht="30">
       <c r="A62" s="7" t="s">
@@ -2212,7 +2230,7 @@
       <c r="D62" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="K62" s="28"/>
+      <c r="K62" s="26"/>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="9"/>
@@ -2225,13 +2243,13 @@
       <c r="D63" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="30"/>
-      <c r="H63" s="30"/>
-      <c r="I63" s="30"/>
-      <c r="J63" s="30"/>
-      <c r="K63" s="32"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="28"/>
+      <c r="J63" s="28"/>
+      <c r="K63" s="30"/>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="7" t="s">
@@ -2246,7 +2264,7 @@
       <c r="D64" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G64" s="28"/>
+      <c r="G64" s="26"/>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="7"/>
@@ -2259,7 +2277,7 @@
       <c r="D65" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="G65" s="28"/>
+      <c r="G65" s="26"/>
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="7"/>
@@ -2272,7 +2290,7 @@
       <c r="D66" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="G66" s="28"/>
+      <c r="G66" s="26"/>
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="7"/>
@@ -2285,10 +2303,10 @@
       <c r="D67" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G67" s="28"/>
+      <c r="G67" s="26"/>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="9"/>
+      <c r="A68" s="10"/>
       <c r="B68" s="9" t="s">
         <v>131</v>
       </c>
@@ -2298,13 +2316,13 @@
       <c r="D68" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
-      <c r="G68" s="32"/>
-      <c r="H68" s="30"/>
-      <c r="I68" s="30"/>
-      <c r="J68" s="30"/>
-      <c r="K68" s="30"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="28"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="28"/>
+      <c r="I68" s="28"/>
+      <c r="J68" s="28"/>
+      <c r="K68" s="28"/>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="7"/>
@@ -2315,139 +2333,177 @@
         <v>134</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="G69" s="28"/>
+        <v>182</v>
+      </c>
+      <c r="G69" s="26"/>
     </row>
     <row r="70" spans="1:11">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E70" s="30"/>
-      <c r="F70" s="30"/>
-      <c r="G70" s="32"/>
-      <c r="H70" s="30"/>
-      <c r="I70" s="30"/>
-      <c r="J70" s="30"/>
-      <c r="K70" s="30"/>
+      <c r="A70" s="7"/>
+      <c r="B70" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G70" s="26"/>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C71" s="13" t="s">
+      <c r="A71" s="7"/>
+      <c r="B71" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D71" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="34"/>
-      <c r="I71" s="31"/>
-      <c r="J71" s="31"/>
-      <c r="K71" s="31"/>
+      <c r="D71" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G71" s="26"/>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="7"/>
-      <c r="B72" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>141</v>
-      </c>
+      <c r="B72" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28"/>
+      <c r="G72" s="30"/>
       <c r="H72" s="28"/>
+      <c r="I72" s="28"/>
+      <c r="J72" s="28"/>
+      <c r="K72" s="28"/>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="7"/>
-      <c r="B73" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C73" s="9" t="s">
+      <c r="A73" s="9"/>
+      <c r="B73" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="C73" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D73" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
-      <c r="G73" s="30"/>
-      <c r="H73" s="32"/>
-      <c r="I73" s="30"/>
-      <c r="J73" s="30"/>
-      <c r="K73" s="30"/>
+      <c r="D73" s="11" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="7"/>
-      <c r="B74" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="D74" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H74" s="28"/>
+      <c r="A74" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="29"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="29"/>
+      <c r="J74" s="29"/>
+      <c r="K74" s="29"/>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="7"/>
       <c r="B75" s="10" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="H75" s="28"/>
+        <v>140</v>
+      </c>
+      <c r="H75" s="26"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="7"/>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E76" s="28"/>
+      <c r="F76" s="28"/>
+      <c r="G76" s="28"/>
+      <c r="H76" s="30"/>
+      <c r="I76" s="28"/>
+      <c r="J76" s="28"/>
+      <c r="K76" s="28"/>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="7"/>
+      <c r="B77" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H77" s="26"/>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="7"/>
+      <c r="B78" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="H78" s="26"/>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="7"/>
+      <c r="B79" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C79" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="D79" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="H79" s="26"/>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="9"/>
+      <c r="B80" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="H76" s="28"/>
-    </row>
-    <row r="77" spans="1:11">
-      <c r="A77" s="9"/>
-      <c r="B77" s="9" t="s">
+      <c r="C80" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="D80" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D77" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E77" s="30"/>
-      <c r="F77" s="30"/>
-      <c r="G77" s="30"/>
-      <c r="H77" s="32"/>
-      <c r="I77" s="30"/>
-      <c r="J77" s="30"/>
-      <c r="K77" s="30"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="28"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="28"/>
+      <c r="J80" s="28"/>
+      <c r="K80" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
added literature mining example
</commit_message>
<xml_diff>
--- a/doc/json_schema_migration_from_1.1_to_1.2.xlsx
+++ b/doc/json_schema_migration_from_1.1_to_1.2.xlsx
@@ -384,9 +384,6 @@
     <t>.evidence.evidence_chain[0].evidence.provenance_type.literature.pubmed_refs</t>
   </si>
   <si>
-    <t>.evidence.target2drug.provenance_type.literature.lit_refs</t>
-  </si>
-  <si>
     <t>Mechanism of action of drug</t>
   </si>
   <si>
@@ -565,6 +562,9 @@
   </si>
   <si>
     <t>.drug.molecule_name</t>
+  </si>
+  <si>
+    <t>.evidence.target2drug.provenance_type.literature.references</t>
   </si>
 </sst>
 </file>
@@ -769,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -835,16 +835,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -854,6 +848,10 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1369,8 +1367,8 @@
   </sheetPr>
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1480,10 +1478,10 @@
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="33.75" customHeight="1">
-      <c r="A12" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="B12" s="33"/>
+      <c r="A12" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="27"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3">
@@ -1492,10 +1490,10 @@
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="21" customHeight="1">
-      <c r="A14" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="B14" s="34"/>
+      <c r="A14" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" s="28"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3">
@@ -1592,19 +1590,19 @@
       <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="30" customHeight="1">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
     </row>
     <row r="27" spans="1:11" ht="177.75">
       <c r="A27" s="23" t="s">
@@ -1619,25 +1617,25 @@
       <c r="D27" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="G27" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="J27" s="27" t="s">
+      <c r="J27" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="27" t="s">
+      <c r="K27" s="25" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1654,13 +1652,13 @@
       <c r="D28" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="7"/>
@@ -1673,13 +1671,13 @@
       <c r="D29" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="7"/>
@@ -1692,13 +1690,13 @@
       <c r="D30" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="7"/>
@@ -1711,13 +1709,13 @@
       <c r="D31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="7"/>
@@ -1730,7 +1728,13 @@
       <c r="D32" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G32" s="26"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="7"/>
@@ -1743,13 +1747,13 @@
       <c r="D33" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="30"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="7"/>
@@ -1762,13 +1766,13 @@
       <c r="D34" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="7"/>
@@ -1781,64 +1785,70 @@
       <c r="D35" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="7"/>
       <c r="B36" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
+        <v>158</v>
+      </c>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="7"/>
       <c r="B37" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="E37" s="26"/>
+        <v>161</v>
+      </c>
+      <c r="E37" s="30"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E38" s="30"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="7"/>
@@ -1851,13 +1861,13 @@
       <c r="D39" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="7"/>
@@ -1870,13 +1880,13 @@
       <c r="D40" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="7"/>
@@ -1889,13 +1899,13 @@
       <c r="D41" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="7"/>
@@ -1908,13 +1918,13 @@
       <c r="D42" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="26"/>
-      <c r="K42" s="26"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="7"/>
@@ -1927,10 +1937,13 @@
       <c r="D43" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="26"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="31"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="7"/>
@@ -1943,15 +1956,17 @@
       <c r="D44" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F44" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="J44" s="25"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="J44" s="32"/>
+      <c r="K44" s="31"/>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="7"/>
@@ -1964,9 +1979,13 @@
       <c r="D45" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="31"/>
     </row>
     <row r="46" spans="1:11" ht="30">
       <c r="A46" s="7"/>
@@ -1979,9 +1998,13 @@
       <c r="D46" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="31"/>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="7"/>
@@ -1994,12 +2017,13 @@
       <c r="D47" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="30"/>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="7"/>
@@ -2012,13 +2036,13 @@
       <c r="D48" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="7"/>
@@ -2031,12 +2055,13 @@
       <c r="D49" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="30"/>
+      <c r="K49" s="30"/>
     </row>
     <row r="50" spans="1:11" ht="30">
       <c r="A50" s="7"/>
@@ -2049,8 +2074,13 @@
       <c r="D50" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="I50" s="26"/>
-      <c r="J50" s="26"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
+      <c r="K50" s="31"/>
     </row>
     <row r="51" spans="1:11" ht="30">
       <c r="A51" s="9"/>
@@ -2063,13 +2093,13 @@
       <c r="D51" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="28"/>
-      <c r="H51" s="28"/>
-      <c r="I51" s="28"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="31"/>
       <c r="J51" s="30"/>
-      <c r="K51" s="28"/>
+      <c r="K51" s="31"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="7" t="s">
@@ -2084,7 +2114,13 @@
       <c r="D52" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E52" s="26"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="31"/>
+      <c r="K52" s="31"/>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="7"/>
@@ -2097,72 +2133,108 @@
       <c r="D53" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="26"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+      <c r="K53" s="31"/>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="7"/>
       <c r="B54" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>105</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E54" s="26"/>
+        <v>169</v>
+      </c>
+      <c r="E54" s="30"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="31"/>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="7"/>
       <c r="B55" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E55" s="26"/>
+        <v>170</v>
+      </c>
+      <c r="E55" s="30"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="31"/>
+      <c r="K55" s="31"/>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="7"/>
       <c r="B56" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E56" s="26"/>
+        <v>171</v>
+      </c>
+      <c r="E56" s="30"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="31"/>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="7"/>
       <c r="B57" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E57" s="26"/>
+        <v>165</v>
+      </c>
+      <c r="E57" s="30"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="31"/>
+      <c r="H57" s="31"/>
+      <c r="I57" s="31"/>
+      <c r="J57" s="31"/>
+      <c r="K57" s="31"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="7"/>
       <c r="B58" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E58" s="26"/>
+        <v>166</v>
+      </c>
+      <c r="E58" s="30"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="31"/>
+      <c r="J58" s="31"/>
+      <c r="K58" s="31"/>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="7"/>
@@ -2175,7 +2247,13 @@
       <c r="D59" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E59" s="26"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="31"/>
+      <c r="K59" s="31"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="9"/>
@@ -2189,12 +2267,12 @@
         <v>110</v>
       </c>
       <c r="E60" s="30"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
-      <c r="H60" s="28"/>
-      <c r="I60" s="28"/>
-      <c r="J60" s="28"/>
-      <c r="K60" s="28"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+      <c r="H60" s="31"/>
+      <c r="I60" s="31"/>
+      <c r="J60" s="31"/>
+      <c r="K60" s="31"/>
     </row>
     <row r="61" spans="1:11" ht="45">
       <c r="A61" s="13" t="s">
@@ -2209,13 +2287,13 @@
       <c r="D61" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E61" s="29"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="29"/>
-      <c r="H61" s="29"/>
-      <c r="I61" s="32"/>
-      <c r="J61" s="29"/>
-      <c r="K61" s="29"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="31"/>
+      <c r="H61" s="31"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="31"/>
+      <c r="K61" s="31"/>
     </row>
     <row r="62" spans="1:11" ht="30">
       <c r="A62" s="7" t="s">
@@ -2230,7 +2308,13 @@
       <c r="D62" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="K62" s="26"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+      <c r="H62" s="31"/>
+      <c r="I62" s="31"/>
+      <c r="J62" s="31"/>
+      <c r="K62" s="30"/>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="9"/>
@@ -2243,12 +2327,12 @@
       <c r="D63" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
-      <c r="G63" s="28"/>
-      <c r="H63" s="28"/>
-      <c r="I63" s="28"/>
-      <c r="J63" s="28"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="31"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="31"/>
       <c r="K63" s="30"/>
     </row>
     <row r="64" spans="1:11">
@@ -2262,248 +2346,321 @@
         <v>121</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G64" s="26"/>
+        <v>182</v>
+      </c>
+      <c r="E64" s="31"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="31"/>
+      <c r="J64" s="31"/>
+      <c r="K64" s="31"/>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="7"/>
       <c r="B65" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="G65" s="26"/>
+        <v>123</v>
+      </c>
+      <c r="E65" s="31"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="31"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="31"/>
+      <c r="K65" s="31"/>
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="7"/>
       <c r="B66" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="D66" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G66" s="26"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="31"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="31"/>
+      <c r="I66" s="31"/>
+      <c r="J66" s="31"/>
+      <c r="K66" s="31"/>
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="7"/>
       <c r="B67" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="D67" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D67" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G67" s="26"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="30"/>
+      <c r="H67" s="31"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="31"/>
+      <c r="K67" s="31"/>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="10"/>
       <c r="B68" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>132</v>
-      </c>
       <c r="D68" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="E68" s="28"/>
-      <c r="F68" s="28"/>
+        <v>129</v>
+      </c>
+      <c r="E68" s="31"/>
+      <c r="F68" s="31"/>
       <c r="G68" s="30"/>
-      <c r="H68" s="28"/>
-      <c r="I68" s="28"/>
-      <c r="J68" s="28"/>
-      <c r="K68" s="28"/>
+      <c r="H68" s="31"/>
+      <c r="I68" s="31"/>
+      <c r="J68" s="31"/>
+      <c r="K68" s="31"/>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="7"/>
       <c r="B69" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C69" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C69" s="10" t="s">
-        <v>134</v>
-      </c>
       <c r="D69" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="G69" s="26"/>
+        <v>181</v>
+      </c>
+      <c r="E69" s="31"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="31"/>
+      <c r="I69" s="31"/>
+      <c r="J69" s="31"/>
+      <c r="K69" s="31"/>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="7"/>
       <c r="B70" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="G70" s="26"/>
+        <v>180</v>
+      </c>
+      <c r="E70" s="31"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="30"/>
+      <c r="H70" s="31"/>
+      <c r="I70" s="31"/>
+      <c r="J70" s="31"/>
+      <c r="K70" s="31"/>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="7"/>
       <c r="B71" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="G71" s="26"/>
+        <v>175</v>
+      </c>
+      <c r="E71" s="31"/>
+      <c r="F71" s="31"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="31"/>
+      <c r="I71" s="31"/>
+      <c r="J71" s="31"/>
+      <c r="K71" s="31"/>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="7"/>
       <c r="B72" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E72" s="28"/>
-      <c r="F72" s="28"/>
+        <v>135</v>
+      </c>
+      <c r="E72" s="31"/>
+      <c r="F72" s="31"/>
       <c r="G72" s="30"/>
-      <c r="H72" s="28"/>
-      <c r="I72" s="28"/>
-      <c r="J72" s="28"/>
-      <c r="K72" s="28"/>
+      <c r="H72" s="31"/>
+      <c r="I72" s="31"/>
+      <c r="J72" s="31"/>
+      <c r="K72" s="31"/>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="9"/>
-      <c r="B73" s="29" t="s">
-        <v>177</v>
+      <c r="B73" s="26" t="s">
+        <v>176</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>95</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>178</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="E73" s="31"/>
+      <c r="F73" s="31"/>
+      <c r="G73" s="30"/>
+      <c r="H73" s="31"/>
+      <c r="I73" s="31"/>
+      <c r="J73" s="31"/>
+      <c r="K73" s="31"/>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>95</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="E74" s="29"/>
-      <c r="F74" s="29"/>
-      <c r="G74" s="29"/>
-      <c r="H74" s="32"/>
-      <c r="I74" s="29"/>
-      <c r="J74" s="29"/>
-      <c r="K74" s="29"/>
+        <v>137</v>
+      </c>
+      <c r="E74" s="31"/>
+      <c r="F74" s="31"/>
+      <c r="G74" s="31"/>
+      <c r="H74" s="30"/>
+      <c r="I74" s="31"/>
+      <c r="J74" s="31"/>
+      <c r="K74" s="31"/>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="7"/>
       <c r="B75" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="H75" s="26"/>
+        <v>139</v>
+      </c>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="31"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="31"/>
+      <c r="K75" s="31"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="7"/>
       <c r="B76" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>95</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E76" s="28"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="28"/>
+        <v>141</v>
+      </c>
+      <c r="E76" s="31"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="31"/>
       <c r="H76" s="30"/>
-      <c r="I76" s="28"/>
-      <c r="J76" s="28"/>
-      <c r="K76" s="28"/>
+      <c r="I76" s="31"/>
+      <c r="J76" s="31"/>
+      <c r="K76" s="31"/>
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="7"/>
       <c r="B77" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C77" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C77" s="10" t="s">
+      <c r="D77" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="D77" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="H77" s="26"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="30"/>
+      <c r="I77" s="31"/>
+      <c r="J77" s="31"/>
+      <c r="K77" s="31"/>
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="7"/>
       <c r="B78" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C78" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C78" s="10" t="s">
+      <c r="D78" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D78" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="H78" s="26"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="31"/>
+      <c r="G78" s="31"/>
+      <c r="H78" s="30"/>
+      <c r="I78" s="31"/>
+      <c r="J78" s="31"/>
+      <c r="K78" s="31"/>
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="7"/>
       <c r="B79" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="D79" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D79" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="H79" s="26"/>
+      <c r="E79" s="31"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="31"/>
+      <c r="H79" s="30"/>
+      <c r="I79" s="31"/>
+      <c r="J79" s="31"/>
+      <c r="K79" s="31"/>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="9"/>
       <c r="B80" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C80" s="9" t="s">
+      <c r="D80" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="D80" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="E80" s="28"/>
-      <c r="F80" s="28"/>
-      <c r="G80" s="28"/>
+      <c r="E80" s="31"/>
+      <c r="F80" s="31"/>
+      <c r="G80" s="31"/>
       <c r="H80" s="30"/>
-      <c r="I80" s="28"/>
-      <c r="J80" s="28"/>
-      <c r="K80" s="28"/>
+      <c r="I80" s="31"/>
+      <c r="J80" s="31"/>
+      <c r="K80" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
renamed genomics -> genetics
</commit_message>
<xml_diff>
--- a/doc/json_schema_migration_from_1.1_to_1.2.xlsx
+++ b/doc/json_schema_migration_from_1.1_to_1.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="182">
   <si>
     <t>Table 1. Types of target-disease 'evidence chains': this field needs to be specified in .type field in the schema</t>
   </si>
@@ -30,9 +30,6 @@
     <t>CTTV006_Networks_Reactome</t>
   </si>
   <si>
-    <t>affected_pathways_evidence_string</t>
-  </si>
-  <si>
     <t>CTTV006_Networks_IntAct</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>CTTV011_UniProt</t>
   </si>
   <si>
-    <t>genetics_literature_evidence_string OR genetics_evidence_string depending on whether dbSNP/ESV/NSV variant IDs are available</t>
-  </si>
-  <si>
     <t>CTTV012_Variation</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>expression</t>
   </si>
   <si>
-    <t>literature_evidence_string, genetics_literature_evidence_string, affected_pathways_evidence_string</t>
-  </si>
-  <si>
     <t>literature</t>
   </si>
   <si>
@@ -321,48 +312,30 @@
     <t>.evidence.experiment_specific.comparison_name</t>
   </si>
   <si>
-    <t>.evidence.expression.comparison_name</t>
-  </si>
-  <si>
     <t>Study details</t>
   </si>
   <si>
     <t>.biological_object.properties.experiment_specific</t>
   </si>
   <si>
-    <t>.evidence.expression.study_details</t>
-  </si>
-  <si>
     <t>.evidence.experiment_specific.log2_fold_change</t>
   </si>
   <si>
     <t>.evidence.association_score.pvalue.value</t>
   </si>
   <si>
-    <t>.evidence.expression.association_score.pvalue.value</t>
-  </si>
-  <si>
     <t>Provenance - References</t>
   </si>
   <si>
     <t>.evidence.experiment_specific.literature.pubmed_refs</t>
   </si>
   <si>
-    <t>.evidence.expression.literature.references</t>
-  </si>
-  <si>
-    <t>literature_evidence_string, genomics_literature_evidence_string, affected_pathways_evidence_string</t>
-  </si>
-  <si>
     <t>Mutations</t>
   </si>
   <si>
     <t>.evidence.properties.experiment_specific.additional_properties</t>
   </si>
   <si>
-    <t>.evidence.literature.known_mutations</t>
-  </si>
-  <si>
     <t>Mouse Phenotypes</t>
   </si>
   <si>
@@ -480,9 +453,6 @@
     <t>.evidence.variant2disease.provenance_type.expert</t>
   </si>
   <si>
-    <t>NOTE: affected_pathways_evidence_string, literature_evidence_string and genetics_literature_evidence_string are the same schema but different valid labels.</t>
-  </si>
-  <si>
     <t>Table 2. Types of 'evidence' objects for linking 2 entities and their corresponding 'evidence chain'</t>
   </si>
   <si>
@@ -513,33 +483,15 @@
     <t>Reference sample</t>
   </si>
   <si>
-    <t>.evidence.expression.reference_sample</t>
-  </si>
-  <si>
-    <t>.evidence.expression.test_sample</t>
-  </si>
-  <si>
     <t>Log2 fold change value</t>
   </si>
   <si>
     <t>Log2 calculation sample size</t>
   </si>
   <si>
-    <t>.evidence.expression.log2_fold_change.value</t>
-  </si>
-  <si>
-    <t>.evidence.expression.log2_fold_change.rank.position</t>
-  </si>
-  <si>
-    <t>.evidence.expression.log2_fold_change.rank.sample_size</t>
-  </si>
-  <si>
     <t>affected_pathways_string</t>
   </si>
   <si>
-    <t>genetics_literature_evidence_string</t>
-  </si>
-  <si>
     <t>=1</t>
   </si>
   <si>
@@ -565,6 +517,51 @@
   </si>
   <si>
     <t>.evidence.target2drug.provenance_type.literature.references</t>
+  </si>
+  <si>
+    <t>.evidence.comparison_name</t>
+  </si>
+  <si>
+    <t>.evidence.study_details</t>
+  </si>
+  <si>
+    <t>.evidence.log2_fold_change.value</t>
+  </si>
+  <si>
+    <t>.evidence.log2_fold_change.rank.position</t>
+  </si>
+  <si>
+    <t>.evidence.log2_fold_change.rank.sample_size</t>
+  </si>
+  <si>
+    <t>.evidence.reference_sample</t>
+  </si>
+  <si>
+    <t>.evidence.test_sample</t>
+  </si>
+  <si>
+    <t>.evidence.literature.references</t>
+  </si>
+  <si>
+    <t>.evidence.known_mutations</t>
+  </si>
+  <si>
+    <t>affected_pathways_curated_literature_evidence_string</t>
+  </si>
+  <si>
+    <t>literature_evidence_string, genomics_literature_evidence_string, affected_pathways_curated_literature_evidence_string</t>
+  </si>
+  <si>
+    <t>genomics_curated_literature_evidence_string OR genetics_evidence_string depending on whether dbSNP/ESV/NSV variant IDs are available</t>
+  </si>
+  <si>
+    <t>NOTE: affected_pathways_curated_literature_evidence_string, literature_evidence_string and genomics_curated_literature_evidence_string are the same schema but different valid labels.</t>
+  </si>
+  <si>
+    <t>literature_evidence_string, genomics_curated_literature_evidence_string, affected_pathways_curated_literature_evidence_string</t>
+  </si>
+  <si>
+    <t>genomics_curated_literature_evidence_string</t>
   </si>
 </sst>
 </file>
@@ -839,6 +836,10 @@
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -848,10 +849,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1367,8 +1364,8 @@
   </sheetPr>
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1401,87 +1398,87 @@
         <v>3</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>4</v>
+        <v>176</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>4</v>
+        <v>176</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>7</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="45">
+      <c r="A7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="30">
-      <c r="A7" s="14" t="s">
-        <v>10</v>
-      </c>
       <c r="B7" s="15" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="33.75" customHeight="1">
-      <c r="A12" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="B12" s="27"/>
+      <c r="A12" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="31"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3">
@@ -1490,99 +1487,99 @@
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="21" customHeight="1">
-      <c r="A14" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14" s="28"/>
+      <c r="A14" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="32"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="45">
+    <row r="19" spans="1:11" ht="75">
       <c r="A19" s="14" t="s">
-        <v>24</v>
+        <v>180</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1590,1077 +1587,1077 @@
       <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="30" customHeight="1">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+    </row>
+    <row r="27" spans="1:11" ht="225">
+      <c r="A27" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-    </row>
-    <row r="27" spans="1:11" ht="177.75">
-      <c r="A27" s="23" t="s">
+      <c r="D27" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>35</v>
-      </c>
       <c r="E27" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="G27" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="J27" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="J27" s="25" t="s">
+      <c r="K27" s="25" t="s">
         <v>16</v>
-      </c>
-      <c r="K27" s="25" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="7"/>
       <c r="B29" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="7"/>
       <c r="B30" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
+        <v>42</v>
+      </c>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="7"/>
       <c r="B31" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="7"/>
       <c r="B32" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
+        <v>48</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="7"/>
       <c r="B33" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C33" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="7"/>
       <c r="B34" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
+        <v>53</v>
+      </c>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="7"/>
       <c r="B35" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
+        <v>56</v>
+      </c>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="7"/>
       <c r="B36" s="7" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
+        <v>148</v>
+      </c>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="7"/>
       <c r="B37" s="6" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="E37" s="30"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
+        <v>151</v>
+      </c>
+      <c r="E37" s="27"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E38" s="30"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="31"/>
+        <v>152</v>
+      </c>
+      <c r="E38" s="27"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="7"/>
       <c r="B39" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
+        <v>60</v>
+      </c>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="7"/>
       <c r="B40" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
+        <v>63</v>
+      </c>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="7"/>
       <c r="B41" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
+        <v>66</v>
+      </c>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="7"/>
       <c r="B42" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
+        <v>69</v>
+      </c>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="7"/>
       <c r="B43" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E43" s="30"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="31"/>
+        <v>72</v>
+      </c>
+      <c r="E43" s="27"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="28"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="7"/>
       <c r="B44" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44" s="31"/>
-      <c r="F44" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="J44" s="32"/>
-      <c r="K44" s="31"/>
+        <v>75</v>
+      </c>
+      <c r="E44" s="28"/>
+      <c r="F44" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="J44" s="29"/>
+      <c r="K44" s="28"/>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="7"/>
       <c r="B45" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="31"/>
+        <v>78</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="28"/>
     </row>
     <row r="46" spans="1:11" ht="30">
       <c r="A46" s="7"/>
       <c r="B46" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="31"/>
+        <v>81</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="28"/>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="7"/>
       <c r="B47" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E47" s="31"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
+        <v>84</v>
+      </c>
+      <c r="E47" s="28"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="27"/>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="7"/>
       <c r="B48" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
+        <v>87</v>
+      </c>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="7"/>
       <c r="B49" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E49" s="31"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
+        <v>90</v>
+      </c>
+      <c r="E49" s="28"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
     </row>
     <row r="50" spans="1:11" ht="30">
       <c r="A50" s="7"/>
       <c r="B50" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="31"/>
+        <v>93</v>
+      </c>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="28"/>
     </row>
     <row r="51" spans="1:11" ht="30">
       <c r="A51" s="9"/>
       <c r="B51" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C51" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D51" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="31"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="31"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="28"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E52" s="30"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="31"/>
-      <c r="I52" s="31"/>
-      <c r="J52" s="31"/>
-      <c r="K52" s="31"/>
+        <v>167</v>
+      </c>
+      <c r="E52" s="27"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="7"/>
       <c r="B53" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E53" s="30"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="31"/>
-      <c r="K53" s="31"/>
+        <v>168</v>
+      </c>
+      <c r="E53" s="27"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="7"/>
       <c r="B54" s="7" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="E54" s="30"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
-      <c r="J54" s="31"/>
-      <c r="K54" s="31"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="7"/>
       <c r="B55" s="7" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="E55" s="30"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
-      <c r="H55" s="31"/>
-      <c r="I55" s="31"/>
-      <c r="J55" s="31"/>
-      <c r="K55" s="31"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28"/>
+      <c r="J55" s="28"/>
+      <c r="K55" s="28"/>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="7"/>
       <c r="B56" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="E56" s="30"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
-      <c r="J56" s="31"/>
-      <c r="K56" s="31"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+      <c r="J56" s="28"/>
+      <c r="K56" s="28"/>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="7"/>
       <c r="B57" s="7" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="E57" s="30"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
-      <c r="J57" s="31"/>
-      <c r="K57" s="31"/>
+        <v>172</v>
+      </c>
+      <c r="E57" s="27"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="7"/>
       <c r="B58" s="7" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E58" s="30"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31"/>
-      <c r="H58" s="31"/>
-      <c r="I58" s="31"/>
-      <c r="J58" s="31"/>
-      <c r="K58" s="31"/>
+        <v>173</v>
+      </c>
+      <c r="E58" s="27"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="28"/>
+      <c r="J58" s="28"/>
+      <c r="K58" s="28"/>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="7"/>
       <c r="B59" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E59" s="30"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="31"/>
-      <c r="I59" s="31"/>
-      <c r="J59" s="31"/>
-      <c r="K59" s="31"/>
+        <v>101</v>
+      </c>
+      <c r="E59" s="27"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="28"/>
+      <c r="I59" s="28"/>
+      <c r="J59" s="28"/>
+      <c r="K59" s="28"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="9"/>
       <c r="B60" s="9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E60" s="30"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31"/>
-      <c r="H60" s="31"/>
-      <c r="I60" s="31"/>
-      <c r="J60" s="31"/>
-      <c r="K60" s="31"/>
-    </row>
-    <row r="61" spans="1:11" ht="45">
+        <v>174</v>
+      </c>
+      <c r="E60" s="27"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="28"/>
+      <c r="I60" s="28"/>
+      <c r="J60" s="28"/>
+      <c r="K60" s="28"/>
+    </row>
+    <row r="61" spans="1:11" ht="60">
       <c r="A61" s="13" t="s">
-        <v>111</v>
+        <v>177</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="E61" s="31"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="31"/>
-      <c r="H61" s="31"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="31"/>
-      <c r="K61" s="31"/>
+        <v>175</v>
+      </c>
+      <c r="E61" s="28"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="28"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="28"/>
+      <c r="K61" s="28"/>
     </row>
     <row r="62" spans="1:11" ht="30">
       <c r="A62" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E62" s="31"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
-      <c r="H62" s="31"/>
-      <c r="I62" s="31"/>
-      <c r="J62" s="31"/>
-      <c r="K62" s="30"/>
+        <v>108</v>
+      </c>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="28"/>
+      <c r="K62" s="27"/>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="9"/>
       <c r="B63" s="9" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
-      <c r="H63" s="31"/>
-      <c r="I63" s="31"/>
-      <c r="J63" s="31"/>
-      <c r="K63" s="30"/>
+        <v>110</v>
+      </c>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="28"/>
+      <c r="J63" s="28"/>
+      <c r="K63" s="27"/>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="E64" s="31"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="31"/>
-      <c r="I64" s="31"/>
-      <c r="J64" s="31"/>
-      <c r="K64" s="31"/>
+        <v>166</v>
+      </c>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="28"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="28"/>
+      <c r="K64" s="28"/>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="7"/>
       <c r="B65" s="10" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E65" s="31"/>
-      <c r="F65" s="31"/>
-      <c r="G65" s="30"/>
-      <c r="H65" s="31"/>
-      <c r="I65" s="31"/>
-      <c r="J65" s="31"/>
-      <c r="K65" s="31"/>
+        <v>114</v>
+      </c>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+      <c r="J65" s="28"/>
+      <c r="K65" s="28"/>
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="7"/>
       <c r="B66" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E66" s="31"/>
-      <c r="F66" s="31"/>
-      <c r="G66" s="30"/>
-      <c r="H66" s="31"/>
-      <c r="I66" s="31"/>
-      <c r="J66" s="31"/>
-      <c r="K66" s="31"/>
+        <v>117</v>
+      </c>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="27"/>
+      <c r="H66" s="28"/>
+      <c r="I66" s="28"/>
+      <c r="J66" s="28"/>
+      <c r="K66" s="28"/>
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="7"/>
       <c r="B67" s="10" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E67" s="31"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="30"/>
-      <c r="H67" s="31"/>
-      <c r="I67" s="31"/>
-      <c r="J67" s="31"/>
-      <c r="K67" s="31"/>
+        <v>120</v>
+      </c>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="28"/>
+      <c r="I67" s="28"/>
+      <c r="J67" s="28"/>
+      <c r="K67" s="28"/>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="10"/>
       <c r="B68" s="9" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E68" s="31"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="30"/>
-      <c r="H68" s="31"/>
-      <c r="I68" s="31"/>
-      <c r="J68" s="31"/>
-      <c r="K68" s="31"/>
+        <v>120</v>
+      </c>
+      <c r="E68" s="28"/>
+      <c r="F68" s="28"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="28"/>
+      <c r="I68" s="28"/>
+      <c r="J68" s="28"/>
+      <c r="K68" s="28"/>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="7"/>
       <c r="B69" s="10" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="30"/>
-      <c r="H69" s="31"/>
-      <c r="I69" s="31"/>
-      <c r="J69" s="31"/>
-      <c r="K69" s="31"/>
+        <v>165</v>
+      </c>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="28"/>
+      <c r="K69" s="28"/>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="7"/>
       <c r="B70" s="10" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
-      <c r="G70" s="30"/>
-      <c r="H70" s="31"/>
-      <c r="I70" s="31"/>
-      <c r="J70" s="31"/>
-      <c r="K70" s="31"/>
+        <v>164</v>
+      </c>
+      <c r="E70" s="28"/>
+      <c r="F70" s="28"/>
+      <c r="G70" s="27"/>
+      <c r="H70" s="28"/>
+      <c r="I70" s="28"/>
+      <c r="J70" s="28"/>
+      <c r="K70" s="28"/>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="7"/>
       <c r="B71" s="10" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="30"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="31"/>
-      <c r="J71" s="31"/>
-      <c r="K71" s="31"/>
+        <v>159</v>
+      </c>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="28"/>
+      <c r="K71" s="28"/>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="7"/>
       <c r="B72" s="9" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E72" s="31"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="30"/>
-      <c r="H72" s="31"/>
-      <c r="I72" s="31"/>
-      <c r="J72" s="31"/>
-      <c r="K72" s="31"/>
+        <v>126</v>
+      </c>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="28"/>
+      <c r="I72" s="28"/>
+      <c r="J72" s="28"/>
+      <c r="K72" s="28"/>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="9"/>
       <c r="B73" s="26" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="E73" s="31"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="30"/>
-      <c r="H73" s="31"/>
-      <c r="I73" s="31"/>
-      <c r="J73" s="31"/>
-      <c r="K73" s="31"/>
+        <v>161</v>
+      </c>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="28"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="28"/>
+      <c r="K73" s="28"/>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E74" s="31"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="30"/>
-      <c r="I74" s="31"/>
-      <c r="J74" s="31"/>
-      <c r="K74" s="31"/>
+        <v>128</v>
+      </c>
+      <c r="E74" s="28"/>
+      <c r="F74" s="28"/>
+      <c r="G74" s="28"/>
+      <c r="H74" s="27"/>
+      <c r="I74" s="28"/>
+      <c r="J74" s="28"/>
+      <c r="K74" s="28"/>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="7"/>
       <c r="B75" s="10" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E75" s="31"/>
-      <c r="F75" s="31"/>
-      <c r="G75" s="31"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="31"/>
-      <c r="J75" s="31"/>
-      <c r="K75" s="31"/>
+        <v>130</v>
+      </c>
+      <c r="E75" s="28"/>
+      <c r="F75" s="28"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="27"/>
+      <c r="I75" s="28"/>
+      <c r="J75" s="28"/>
+      <c r="K75" s="28"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="7"/>
       <c r="B76" s="9" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E76" s="31"/>
-      <c r="F76" s="31"/>
-      <c r="G76" s="31"/>
-      <c r="H76" s="30"/>
-      <c r="I76" s="31"/>
-      <c r="J76" s="31"/>
-      <c r="K76" s="31"/>
+        <v>132</v>
+      </c>
+      <c r="E76" s="28"/>
+      <c r="F76" s="28"/>
+      <c r="G76" s="28"/>
+      <c r="H76" s="27"/>
+      <c r="I76" s="28"/>
+      <c r="J76" s="28"/>
+      <c r="K76" s="28"/>
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="7"/>
       <c r="B77" s="10" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="E77" s="31"/>
-      <c r="F77" s="31"/>
-      <c r="G77" s="31"/>
-      <c r="H77" s="30"/>
-      <c r="I77" s="31"/>
-      <c r="J77" s="31"/>
-      <c r="K77" s="31"/>
+        <v>135</v>
+      </c>
+      <c r="E77" s="28"/>
+      <c r="F77" s="28"/>
+      <c r="G77" s="28"/>
+      <c r="H77" s="27"/>
+      <c r="I77" s="28"/>
+      <c r="J77" s="28"/>
+      <c r="K77" s="28"/>
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="7"/>
       <c r="B78" s="10" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
-      <c r="H78" s="30"/>
-      <c r="I78" s="31"/>
-      <c r="J78" s="31"/>
-      <c r="K78" s="31"/>
+        <v>138</v>
+      </c>
+      <c r="E78" s="28"/>
+      <c r="F78" s="28"/>
+      <c r="G78" s="28"/>
+      <c r="H78" s="27"/>
+      <c r="I78" s="28"/>
+      <c r="J78" s="28"/>
+      <c r="K78" s="28"/>
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="7"/>
       <c r="B79" s="7" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E79" s="31"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="31"/>
-      <c r="H79" s="30"/>
-      <c r="I79" s="31"/>
-      <c r="J79" s="31"/>
-      <c r="K79" s="31"/>
+        <v>141</v>
+      </c>
+      <c r="E79" s="28"/>
+      <c r="F79" s="28"/>
+      <c r="G79" s="28"/>
+      <c r="H79" s="27"/>
+      <c r="I79" s="28"/>
+      <c r="J79" s="28"/>
+      <c r="K79" s="28"/>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="9"/>
       <c r="B80" s="9" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E80" s="31"/>
-      <c r="F80" s="31"/>
-      <c r="G80" s="31"/>
-      <c r="H80" s="30"/>
-      <c r="I80" s="31"/>
-      <c r="J80" s="31"/>
-      <c r="K80" s="31"/>
+        <v>144</v>
+      </c>
+      <c r="E80" s="28"/>
+      <c r="F80" s="28"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="27"/>
+      <c r="I80" s="28"/>
+      <c r="J80" s="28"/>
+      <c r="K80" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>